<commit_message>
5. Tách các component riêng biệt
</commit_message>
<xml_diff>
--- a/Note.xlsx
+++ b/Note.xlsx
@@ -18,15 +18,60 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>uppercase là ràng buộc nội suy (interpolation)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Pipes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> là một cách rất tốt để format string, tiền tệ, ngày tháng hay những dữ liệu để hiển thị</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Xem thêm về pipes: https://angular.io/guide/pipes</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +112,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>113400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="190500"/>
+          <a:ext cx="7200000" cy="4695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +420,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B28:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="3" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>